<commit_message>
hiyerarşi ve yorum düzenlemeleri
proje tamamlandı. belgede yazan ilk iki tablo oluşturulmalı, setter getter fonksiyonlar oluşturulmalı. Ek olarak test yapılması gerek (ben biraz yaptım herhangi bir hata göremedim ancak daha fazla teste ihtiyacımız var)
</commit_message>
<xml_diff>
--- a/data/lessons/BLM001/grades.xlsx
+++ b/data/lessons/BLM001/grades.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,20 +451,15 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Quiz</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>Vize</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Fin</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>ORT</t>
         </is>
@@ -481,15 +476,12 @@
         <v>100</v>
       </c>
       <c r="D2" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="E2" t="n">
         <v>100</v>
       </c>
       <c r="F2" t="n">
-        <v>100</v>
-      </c>
-      <c r="G2" t="n">
         <v>99</v>
       </c>
     </row>
@@ -504,15 +496,12 @@
         <v>60</v>
       </c>
       <c r="D3" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="E3" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F3" t="n">
-        <v>60</v>
-      </c>
-      <c r="G3" t="n">
         <v>60</v>
       </c>
     </row>
@@ -527,15 +516,12 @@
         <v>50</v>
       </c>
       <c r="D4" t="n">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="E4" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F4" t="n">
-        <v>60</v>
-      </c>
-      <c r="G4" t="n">
         <v>48.3</v>
       </c>
     </row>
@@ -544,90 +530,18 @@
         <v>210501014</v>
       </c>
       <c r="B5" t="n">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="C5" t="n">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="D5" t="n">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="F5" t="n">
-        <v>100</v>
-      </c>
-      <c r="G5" t="n">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>220000306</v>
-      </c>
-      <c r="B6" t="n">
-        <v>70</v>
-      </c>
-      <c r="C6" t="n">
-        <v>60</v>
-      </c>
-      <c r="D6" t="n">
-        <v>80</v>
-      </c>
-      <c r="E6" t="n">
-        <v>50</v>
-      </c>
-      <c r="F6" t="n">
-        <v>60</v>
-      </c>
-      <c r="G6" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>230231501</v>
-      </c>
-      <c r="B7" t="n">
-        <v>10</v>
-      </c>
-      <c r="C7" t="n">
-        <v>50</v>
-      </c>
-      <c r="D7" t="n">
-        <v>33</v>
-      </c>
-      <c r="E7" t="n">
-        <v>50</v>
-      </c>
-      <c r="F7" t="n">
-        <v>60</v>
-      </c>
-      <c r="G7" t="n">
-        <v>48.3</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>248512634</v>
-      </c>
-      <c r="B8" t="n">
-        <v>100</v>
-      </c>
-      <c r="C8" t="n">
-        <v>100</v>
-      </c>
-      <c r="D8" t="n">
-        <v>90</v>
-      </c>
-      <c r="E8" t="n">
-        <v>100</v>
-      </c>
-      <c r="F8" t="n">
-        <v>100</v>
-      </c>
-      <c r="G8" t="n">
         <v>99</v>
       </c>
     </row>

</xml_diff>